<commit_message>
Selenium Season 1 notes and programs till Feb 17th
</commit_message>
<xml_diff>
--- a/HTML Components.xlsx
+++ b/HTML Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM5thDecWS\SeleniumSeasons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21BC3203-4D22-46BF-B0BD-25E5B4BB62A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C40FC6-4F58-4D5E-A67F-F71A1FB4E279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60262C71-2123-485A-827D-C531F4463DD6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>HTML Component</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>item in dropdown</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -458,7 +467,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
@@ -513,10 +522,18 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>

</xml_diff>